<commit_message>
added graphs pure project requirements
</commit_message>
<xml_diff>
--- a/data/hysys_vals.xlsx
+++ b/data/hysys_vals.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="40" documentId="11_F25DC773A252ABDACC10482C611C5E3A5ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C9555F6-EB6B-4EE1-945D-979D5CBAA7CF}"/>
   <bookViews>
-    <workbookView xWindow="33591" yWindow="-6471" windowWidth="17743" windowHeight="15360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35846" yWindow="-3703" windowWidth="13885" windowHeight="23983" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ternary" sheetId="1" r:id="rId1"/>
@@ -116,6 +116,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>